<commit_message>
Adjusment - search title Google Scholar
</commit_message>
<xml_diff>
--- a/article_template.xlsx
+++ b/article_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/thayra_pedroso_sap_com/Documents/Mestrado/snowballing-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{E349D766-73F6-4F44-93ED-AB74844B99A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA4AFA1E-B912-A344-B580-ABE5C39F9D8B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E349D766-73F6-4F44-93ED-AB74844B99A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24615A78-CBF0-E343-BDD1-BBFFB47FE8ED}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Article Title</t>
   </si>
@@ -53,6 +53,171 @@
   </si>
   <si>
     <t>Compliance Management of IaC-Based Cloud Deployments During Runtime</t>
+  </si>
+  <si>
+    <t>Towards a Semantically Useful Definition of Conformance with a Reference Model</t>
+  </si>
+  <si>
+    <t>Detecting and Resolving Coupling-Related Infrastructure as Code Based Architecture Smells in Microservice Deployments</t>
+  </si>
+  <si>
+    <t>Correct-By-Construction Microservices with Model-Driven Engineering</t>
+  </si>
+  <si>
+    <t>A Security Compliance-by-Design Framework Utilizing Reusable Formal Models</t>
+  </si>
+  <si>
+    <t>Detection Strategies for Microservice Security Tactics</t>
+  </si>
+  <si>
+    <t>CALint: a Tool for Enforcing the Clean Architecture’s Dependency Rule in Python</t>
+  </si>
+  <si>
+    <t>Formalization of the AADL Run-Time Services</t>
+  </si>
+  <si>
+    <t>Assessing Architecture Conformance to Coupling-Related Infrastructure-as-Code Best Practices: Metrics and Case Studies</t>
+  </si>
+  <si>
+    <t>Assessing Architecture Conformance to Security-Related Practices in Infrastructure as Code Based Deployments</t>
+  </si>
+  <si>
+    <t>Conformance assessment of Architectural Design Decisions on API endpoint designs derived from domain models</t>
+  </si>
+  <si>
+    <t>Architecture violations detection and visualization in the continuous integration pipeline</t>
+  </si>
+  <si>
+    <t>A Two-Level Approach Based on Model Checking to Support Architecture Conformance Checking</t>
+  </si>
+  <si>
+    <t>Applying a Multi-platform Architectural Conformance Solution in a Real-world Microservice-based System</t>
+  </si>
+  <si>
+    <t>ArchPython: architecture conformance checking for Python systems</t>
+  </si>
+  <si>
+    <t>Enforcing Architectural Security Decisions</t>
+  </si>
+  <si>
+    <t>Monitoring Behavioral Compliance with Architectural Patterns Based on Complex Event Processing</t>
+  </si>
+  <si>
+    <t>Formal specification and verification of reusable communication models for distributed systems architecture</t>
+  </si>
+  <si>
+    <t>On the verification of mission-related properties in software-intensive systems-of-systems architectural design</t>
+  </si>
+  <si>
+    <t>Detecting Architectural Issues During the Continuous Integration Pipeline</t>
+  </si>
+  <si>
+    <t>Discovering Architectural Rules in Practice</t>
+  </si>
+  <si>
+    <t>Formalizing Architectural Rules with Ontologies - An Industrial Evaluation</t>
+  </si>
+  <si>
+    <t>Automated design tests to check Hibernate design recommendations</t>
+  </si>
+  <si>
+    <t>Architectural and Behavioral Analysis for Cyber Security</t>
+  </si>
+  <si>
+    <t>Source-Code Divergence Diagnosis Using Constraints and Cryptography</t>
+  </si>
+  <si>
+    <t>Architecture conformance analysis using model-based testing: A case study approach</t>
+  </si>
+  <si>
+    <t>Identifying Software Architecture Erosion Through Code Comments</t>
+  </si>
+  <si>
+    <t>A Secure Testing Based Approach for Mapreduce Frameworks</t>
+  </si>
+  <si>
+    <t>Formalizing Reusable Communication Models for Distributed Systems Architecture</t>
+  </si>
+  <si>
+    <t>An Ontology-Based Approach for Documenting and Validating Architecture Rules</t>
+  </si>
+  <si>
+    <t>On the Understandability of Semantic Constraints for Behavioral Software Architecture Compliance: A Controlled Experiment</t>
+  </si>
+  <si>
+    <t>Preventing Erosion in Exception Handling Design Using Static-Architecture Conformance Checking</t>
+  </si>
+  <si>
+    <t>A Holistic Approach for Managed Evolution of Automotive Software Product Line Architectures</t>
+  </si>
+  <si>
+    <t>On Adequate Behavior-Based Architecture Conformance Checks</t>
+  </si>
+  <si>
+    <t>Software Architecture Reconstruction and Compliance Checking A Case Study</t>
+  </si>
+  <si>
+    <t>The accuracy of dependency analysis in static architecture compliance checking</t>
+  </si>
+  <si>
+    <t>DCL 2.0: modular and reusable specification of architectural constraints</t>
+  </si>
+  <si>
+    <t>Architecture Conformance Checking with Description Logics</t>
+  </si>
+  <si>
+    <t>Architectural design of a LMS with LTSA-conformance</t>
+  </si>
+  <si>
+    <t>Ensuring and Assessing Architecture Conformance to Microservice Decomposition Patterns</t>
+  </si>
+  <si>
+    <t>Checking sysML models for co-simulation</t>
+  </si>
+  <si>
+    <t>Modular Specification of Architectural Constraints</t>
+  </si>
+  <si>
+    <t>Evaluating an Architecture Conformance Monitoring Solution</t>
+  </si>
+  <si>
+    <t>Behavior-Based Architecture Reconstruction and Conformance Checking</t>
+  </si>
+  <si>
+    <t>A Genetic Approach to Architectural Pattern Discovery</t>
+  </si>
+  <si>
+    <t>Architectural Pattern Definition for Semantically Rich Modular Architectures</t>
+  </si>
+  <si>
+    <t>Dependency Related Parameters in the Reconstruction of a Layered Software Architecture</t>
+  </si>
+  <si>
+    <t>Rule Type Based Reasoning On Architecture Violations: A Case Study</t>
+  </si>
+  <si>
+    <t>Preserving architectural decisions through architectural patterns</t>
+  </si>
+  <si>
+    <t>A Unified Approach to Automatic Testing of Architectural Constraints</t>
+  </si>
+  <si>
+    <t>A Unified Approach to Architecture Conformance Checking</t>
+  </si>
+  <si>
+    <t>Preventing Software Architecture Erosion Through Static Architecture Conformance Checking</t>
+  </si>
+  <si>
+    <t>Automatic translation of architecture constraint specifications into components</t>
+  </si>
+  <si>
+    <t>Dependency Types and Subtypes in the Context of Architecture Reconstruction and Compliance Checking</t>
+  </si>
+  <si>
+    <t>OrionPlanning: Improving Modularization and Checking Consistency on Software Architecture</t>
+  </si>
+  <si>
+    <t>A recommendation system for repairing violations detected by static architecture conformance checking</t>
   </si>
 </sst>
 </file>
@@ -427,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -493,6 +658,281 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>